<commit_message>
add pere mere remove prenom postnom
</commit_message>
<xml_diff>
--- a/public/models/FICHE D'IDENTIFICATION CENK 1e-PRIMAIRE.xlsx
+++ b/public/models/FICHE D'IDENTIFICATION CENK 1e-PRIMAIRE.xlsx
@@ -98,7 +98,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>Lubumbashi, le 08/03/2017</t>
+    <t>Lubumbashi,  08/03/2017</t>
   </si>
   <si>
     <t>SAMBA MUKWAT</t>
@@ -122,7 +122,7 @@
     <t>M</t>
   </si>
   <si>
-    <t>Lubumbashi, le 23/06/2017</t>
+    <t>Lubumbashi,  23/06/2017</t>
   </si>
   <si>
     <t>NGOY SHIMBI Pierre</t>
@@ -158,7 +158,7 @@
     <t>KISIMBA SANGAJI FRANCOISE</t>
   </si>
   <si>
-    <t>Kamina,le 23/11/2017</t>
+    <t>Kamina, 23/11/2017</t>
   </si>
   <si>
     <t>UMBA NKULU Prosper</t>
@@ -176,7 +176,7 @@
     <t>KUNGWA MUKEINA KEMUEL</t>
   </si>
   <si>
-    <t>Lubumbashi,28/02/2017</t>
+    <t>Lubumbashi, 28/02/2017</t>
   </si>
   <si>
     <t>NGOY MUYUMBA Taty</t>
@@ -197,7 +197,7 @@
     <t>SANGA ILUNGA BENICIELLE</t>
   </si>
   <si>
-    <t>Lubumbashi,19/12/2017</t>
+    <t>Lubumbashi, 19/12/2017</t>
   </si>
   <si>
     <t>MULIMBI Jephté</t>
@@ -212,7 +212,7 @@
     <t>NGOIE MOREGA BEYERS</t>
   </si>
   <si>
-    <t>Lubumbashi, le 30/10/2017</t>
+    <t>Lubumbashi, 30/10/2017</t>
   </si>
   <si>
     <t>BEYERS Decker</t>
@@ -227,7 +227,7 @@
     <t>KAKWAT KALAU MERVEDI</t>
   </si>
   <si>
-    <t>Lubumbashi,30/09/2017</t>
+    <t>Lubumbashi, 30/09/2017</t>
   </si>
   <si>
     <t>KAKWAT Kalau</t>
@@ -260,7 +260,7 @@
     <t>BIABU MWABILAYI SHEKINAH</t>
   </si>
   <si>
-    <t>Lubumbashi, le23/11/2016</t>
+    <t>Lubumbashi, 23/11/2016</t>
   </si>
   <si>
     <t>MWABILAYI Jonathan</t>
@@ -1589,8 +1589,8 @@
   <sheetPr/>
   <dimension ref="A1:IG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>

</xml_diff>